<commit_message>
Atualização do power point
</commit_message>
<xml_diff>
--- a/Documentacao/Documentacao/PlanilhaDeAlertas.xlsx
+++ b/Documentacao/Documentacao/PlanilhaDeAlertas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Project2nd\Documentacao\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projeto de PI\Project2nd\Documentacao\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Limite</t>
   </si>
@@ -127,13 +127,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -453,7 +453,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -464,11 +464,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -513,11 +513,11 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -534,8 +534,8 @@
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6">
-        <v>0.9</v>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -545,19 +545,19 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="6">
-        <v>1</v>
+      <c r="D9" s="4">
+        <v>0.81</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
@@ -574,7 +574,7 @@
       <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="s">
@@ -585,7 +585,7 @@
       <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>0.81</v>
       </c>
       <c r="E14" t="s">

</xml_diff>